<commit_message>
Improve params default settings
</commit_message>
<xml_diff>
--- a/portfolio/optimization/OpenBB_Portfolio_Template v1.0.0.xlsx
+++ b/portfolio/optimization/OpenBB_Portfolio_Template v1.0.0.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenbouma/Documents/OpenBB Dany/portfolio/optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCD279F-9DC9-7B4F-89F2-CCA7CD174FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B8DC2-9A76-FE40-8280-D7B491ABE685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{4E6A10D7-C95B-B048-9E7D-368AD146FDA2}"/>
+    <workbookView xWindow="-38400" yWindow="-360" windowWidth="38400" windowHeight="21600" xr2:uid="{4E6A10D7-C95B-B048-9E7D-368AD146FDA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimization" sheetId="1" r:id="rId1"/>
-    <sheet name="CONFIG" sheetId="4" state="hidden" r:id="rId2"/>
+    <sheet name="CONFIG" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Config">CONFIG!$A:$R</definedName>
@@ -2729,9 +2729,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -2779,6 +2776,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3173,7 +3173,7 @@
   <dimension ref="A1:XFC57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3193,16 +3193,16 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="2:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="29"/>
+      <c r="D2" s="41"/>
     </row>
     <row r="3" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>78</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -3216,7 +3216,7 @@
       <c r="B4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>122</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -3231,7 +3231,7 @@
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="9" t="s">
         <v>47</v>
       </c>
@@ -3244,7 +3244,7 @@
       <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -3272,7 +3272,7 @@
       <c r="B8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -3287,7 +3287,7 @@
       <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>0.05</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -3302,7 +3302,7 @@
       <c r="B10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="33">
         <v>0.3</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -3317,7 +3317,7 @@
       <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -3332,7 +3332,7 @@
       <c r="B12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -3347,7 +3347,7 @@
       <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="35">
         <v>0.05</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -3359,7 +3359,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="37"/>
+      <c r="C14" s="36"/>
       <c r="E14" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B14,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
         <v/>
@@ -3369,7 +3369,7 @@
       <c r="B15" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="29" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -3384,8 +3384,8 @@
       <c r="B16" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="38" t="s">
-        <v>87</v>
+      <c r="C16" s="37" t="s">
+        <v>118</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>117</v>
@@ -3396,7 +3396,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="37"/>
+      <c r="C17" s="36"/>
       <c r="E17" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B17,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
         <v/>
@@ -3406,7 +3406,7 @@
       <c r="B18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="29" t="s">
         <v>78</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -3421,7 +3421,7 @@
       <c r="B19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="30" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -3436,7 +3436,7 @@
       <c r="B20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="33">
         <v>-1</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -3444,14 +3444,14 @@
       </c>
       <c r="E20" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B20,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <v>-1</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -3459,14 +3459,14 @@
       </c>
       <c r="E21" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B21,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="68" x14ac:dyDescent="0.2">
       <c r="B22" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="10" t="s">
@@ -3474,14 +3474,14 @@
       </c>
       <c r="E22" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B22,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="204" x14ac:dyDescent="0.2">
       <c r="B23" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -3489,14 +3489,14 @@
       </c>
       <c r="E23" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B23,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="33">
+      <c r="C24" s="32">
         <v>0.94</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -3504,14 +3504,14 @@
       </c>
       <c r="E24" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B24,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>1</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -3526,7 +3526,7 @@
       <c r="B26" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="31">
         <v>0</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -3541,7 +3541,7 @@
       <c r="B27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <v>1</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -3549,14 +3549,14 @@
       </c>
       <c r="E27" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B27,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="31">
         <v>100</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -3571,7 +3571,7 @@
       <c r="B29" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="31">
         <v>123</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -3586,7 +3586,7 @@
       <c r="B30" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="39">
+      <c r="C30" s="38">
         <v>0</v>
       </c>
       <c r="D30" s="11" t="s">
@@ -3599,7 +3599,7 @@
     </row>
     <row r="31" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="37"/>
+      <c r="C31" s="36"/>
       <c r="E31" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B31,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
         <v/>
@@ -3609,7 +3609,7 @@
       <c r="B32" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="29" t="s">
         <v>78</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -3624,7 +3624,7 @@
       <c r="B33" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="12" t="s">
         <v>66</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="B34" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -3652,7 +3652,7 @@
       <c r="B35" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="39">
+      <c r="C35" s="38">
         <v>1</v>
       </c>
       <c r="D35" s="11" t="s">
@@ -3664,7 +3664,7 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="37"/>
+      <c r="C36" s="36"/>
       <c r="E36" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B36,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
         <v/>
@@ -3674,7 +3674,7 @@
       <c r="B37" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D37" s="27" t="s">
@@ -3689,46 +3689,46 @@
       <c r="B38" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="41"/>
+      <c r="C38" s="40"/>
       <c r="D38" s="25" t="s">
         <v>109</v>
       </c>
       <c r="E38" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B38,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="32"/>
+      <c r="C39" s="31"/>
       <c r="D39" s="9" t="s">
         <v>110</v>
       </c>
       <c r="E39" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B39,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="32"/>
+      <c r="C40" s="31"/>
       <c r="D40" s="9" t="s">
         <v>111</v>
       </c>
       <c r="E40" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B40,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="32">
+      <c r="C41" s="31">
         <v>1</v>
       </c>
       <c r="D41" s="9" t="s">
@@ -3736,14 +3736,14 @@
       </c>
       <c r="E41" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B41,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="39">
+      <c r="C42" s="38">
         <v>1</v>
       </c>
       <c r="D42" s="11" t="s">
@@ -3751,11 +3751,11 @@
       </c>
       <c r="E42" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B42,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="37"/>
+      <c r="C43" s="36"/>
       <c r="E43" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B43,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
         <v/>
@@ -3765,7 +3765,7 @@
       <c r="B44" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="30" t="s">
+      <c r="C44" s="29" t="s">
         <v>78</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -3780,7 +3780,7 @@
       <c r="B45" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="30" t="s">
         <v>26</v>
       </c>
       <c r="D45" s="8" t="s">
@@ -3795,7 +3795,7 @@
       <c r="B46" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="32">
+      <c r="C46" s="31">
         <v>100</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -3810,7 +3810,7 @@
       <c r="B47" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C47" s="32">
+      <c r="C47" s="31">
         <f>C46</f>
         <v>100</v>
       </c>
@@ -3826,7 +3826,7 @@
       <c r="B48" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="33">
+      <c r="C48" s="32">
         <f>C13</f>
         <v>0.05</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="B49" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="31" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="13" t="s">
@@ -3857,7 +3857,7 @@
       <c r="B50" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="32">
+      <c r="C50" s="31">
         <f>C51</f>
         <v>10</v>
       </c>
@@ -3873,7 +3873,7 @@
       <c r="B51" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C51" s="32">
+      <c r="C51" s="31">
         <v>10</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -3888,7 +3888,7 @@
       <c r="B52" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="32" t="s">
+      <c r="C52" s="31" t="s">
         <v>37</v>
       </c>
       <c r="D52" s="10" t="s">
@@ -3903,7 +3903,7 @@
       <c r="B53" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="33">
+      <c r="C53" s="32">
         <v>0.05</v>
       </c>
       <c r="D53" s="9" t="s">
@@ -3918,7 +3918,7 @@
       <c r="B54" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="32">
+      <c r="C54" s="31">
         <v>1</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -3933,7 +3933,7 @@
       <c r="B55" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="C55" s="38" t="s">
         <v>43</v>
       </c>
       <c r="D55" s="14" t="s">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="E55" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B55,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2"/>
@@ -4014,8 +4014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E3BDC-4C34-1144-B007-DAE78D4AEBEB}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5843,7 +5843,7 @@
         <v>84</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="N32" s="17" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Update Portfolios and Params sheets
</commit_message>
<xml_diff>
--- a/portfolio/optimization/OpenBB_Portfolio_Template v1.0.0.xlsx
+++ b/portfolio/optimization/OpenBB_Portfolio_Template v1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenbouma/Documents/OpenBB Dany/portfolio/optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B8DC2-9A76-FE40-8280-D7B491ABE685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40399F8E-A5B9-E64C-ACD7-B8E86AA22083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-360" windowWidth="38400" windowHeight="21600" xr2:uid="{4E6A10D7-C95B-B048-9E7D-368AD146FDA2}"/>
   </bookViews>
@@ -2647,7 +2647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2779,6 +2779,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3172,8 +3176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D68F2FA-964B-DB41-A4DF-DD4A2F7AD4F5}">
   <dimension ref="A1:XFC57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3385,7 +3389,7 @@
         <v>79</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>117</v>
@@ -3436,7 +3440,7 @@
       <c r="B20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="42">
         <v>-1</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -3444,7 +3448,7 @@
       </c>
       <c r="E20" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B20,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -3459,7 +3463,7 @@
       </c>
       <c r="E21" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B21,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="68" x14ac:dyDescent="0.2">
@@ -3474,7 +3478,7 @@
       </c>
       <c r="E22" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B22,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="204" x14ac:dyDescent="0.2">
@@ -3489,7 +3493,7 @@
       </c>
       <c r="E23" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B23,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -3504,7 +3508,7 @@
       </c>
       <c r="E24" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B24,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
@@ -3549,7 +3553,7 @@
       </c>
       <c r="E27" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B27,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
@@ -3695,7 +3699,7 @@
       </c>
       <c r="E38" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B38,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
@@ -3708,7 +3712,7 @@
       </c>
       <c r="E39" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B39,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
@@ -3721,7 +3725,7 @@
       </c>
       <c r="E40" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B40,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
@@ -3736,7 +3740,7 @@
       </c>
       <c r="E41" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B41,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3751,7 +3755,7 @@
       </c>
       <c r="E42" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B42,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3941,13 +3945,13 @@
       </c>
       <c r="E55" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B55,CONFIG!$B:$Z,MATCH($C$16,CONFIG!$B$1:$Z$1,0),FALSE),"")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="C2:D2"/>

</xml_diff>